<commit_message>
Aggiornato il file report-checklist.xlsx
Aggiornato il file report-checklist.xlsx secondo le istruzioni indicate nella pull request #2062
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#WERFENXX/instrumentation-laboratory-spa/parmagts/12/report-checklist.xlsx
+++ b/GATEWAY/A1#111#WERFENXX/instrumentation-laboratory-spa/parmagts/12/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgrandi\OneDrive - Werfen\Documentos\_IMPIANTI\TORINO\TO4 FSE\FSE Accreditamento LAB\A1#111#WERFENXX\instrumentation-laboratory-spa\parmagts\12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50542B90-5430-4BC1-A146-1929EDFF6853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1928A7B-52FA-4677-8E77-62BFBD8EFA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="516">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1936,9 +1936,6 @@
     <t>In caso di timeout l'esecuzione prosegue ed il referto viene prodotto correttamente. Il re-invio viene eseguito mediante code di gestione che eseguono nuovi tentativi (max 5). L'utente può visualizzare l'esito  dell'invio a FSE. L'utente può effettuare un nuovo invio.</t>
   </si>
   <si>
-    <t>campo valorizzato di default</t>
-  </si>
-  <si>
     <t>L'applicativo non effettua esami rpetuti</t>
   </si>
   <si>
@@ -1985,6 +1982,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4c5ee8a0606f45ee3cd66155a7c9902de377bd7321bc446002c23bf880f14e15.16d607abd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>In caso di errore l'esecuzione prosegue ed il referto viene prodotto correttamente. L'utente può visualizzare l'esito dell'invio a FSE. L'utente può correggere l'errore ed effettuare un nuovo invio.</t>
   </si>
 </sst>
 </file>
@@ -4386,10 +4386,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S191" sqref="S191"/>
+      <selection pane="bottomRight" activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4875,7 +4875,7 @@
         <v>318</v>
       </c>
       <c r="L14" s="34" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
@@ -5510,7 +5510,7 @@
         <v>318</v>
       </c>
       <c r="L31" s="71" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
@@ -5812,7 +5812,7 @@
         <v>318</v>
       </c>
       <c r="L39" s="71" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M39" s="34"/>
       <c r="N39" s="34"/>
@@ -6437,13 +6437,13 @@
         <v>45793</v>
       </c>
       <c r="G55" s="33" t="s">
+        <v>505</v>
+      </c>
+      <c r="H55" s="33" t="s">
         <v>506</v>
       </c>
-      <c r="H55" s="33" t="s">
+      <c r="I55" s="33" t="s">
         <v>507</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>508</v>
       </c>
       <c r="J55" s="34" t="s">
         <v>87</v>
@@ -6457,14 +6457,20 @@
         <v>87</v>
       </c>
       <c r="O55" s="72" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="P55" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="Q55" s="34"/>
-      <c r="R55" s="34"/>
-      <c r="S55" s="34"/>
+      <c r="Q55" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="R55" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="S55" s="34" t="s">
+        <v>515</v>
+      </c>
       <c r="T55" s="34" t="s">
         <v>305</v>
       </c>
@@ -6494,13 +6500,13 @@
         <v>45793</v>
       </c>
       <c r="G56" s="33" t="s">
+        <v>508</v>
+      </c>
+      <c r="H56" s="33" t="s">
         <v>509</v>
       </c>
-      <c r="H56" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>510</v>
-      </c>
-      <c r="I56" s="33" t="s">
-        <v>511</v>
       </c>
       <c r="J56" s="34" t="s">
         <v>87</v>
@@ -6514,14 +6520,20 @@
         <v>87</v>
       </c>
       <c r="O56" s="72" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="P56" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="Q56" s="34"/>
-      <c r="R56" s="34"/>
-      <c r="S56" s="34"/>
+      <c r="Q56" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="R56" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="S56" s="34" t="s">
+        <v>515</v>
+      </c>
       <c r="T56" s="34" t="s">
         <v>305</v>
       </c>
@@ -6592,13 +6604,13 @@
         <v>45793</v>
       </c>
       <c r="G58" s="33" t="s">
+        <v>511</v>
+      </c>
+      <c r="H58" s="33" t="s">
         <v>512</v>
       </c>
-      <c r="H58" s="33" t="s">
+      <c r="I58" s="33" t="s">
         <v>513</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>514</v>
       </c>
       <c r="J58" s="34" t="s">
         <v>87</v>
@@ -6612,14 +6624,20 @@
         <v>87</v>
       </c>
       <c r="O58" s="72" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="P58" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="Q58" s="34"/>
-      <c r="R58" s="34"/>
-      <c r="S58" s="34"/>
+      <c r="Q58" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="R58" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="S58" s="34" t="s">
+        <v>515</v>
+      </c>
       <c r="T58" s="34" t="s">
         <v>305</v>
       </c>
@@ -6735,7 +6753,7 @@
         <v>307</v>
       </c>
       <c r="K61" s="34" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="34"/>
@@ -6776,7 +6794,7 @@
         <v>307</v>
       </c>
       <c r="K62" s="34" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="34"/>
@@ -6817,7 +6835,7 @@
         <v>307</v>
       </c>
       <c r="K63" s="34" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="L63" s="34"/>
       <c r="M63" s="34"/>
@@ -6858,7 +6876,7 @@
         <v>307</v>
       </c>
       <c r="K64" s="34" t="s">
-        <v>499</v>
+        <v>314</v>
       </c>
       <c r="L64" s="34"/>
       <c r="M64" s="34"/>
@@ -11533,7 +11551,7 @@
         <v>318</v>
       </c>
       <c r="L190" s="34" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M190" s="34"/>
       <c r="N190" s="34"/>
@@ -11569,13 +11587,13 @@
         <v>45824</v>
       </c>
       <c r="G191" s="33" t="s">
+        <v>503</v>
+      </c>
+      <c r="H191" s="33" t="s">
         <v>504</v>
       </c>
-      <c r="H191" s="33" t="s">
-        <v>505</v>
-      </c>
       <c r="I191" s="33" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J191" s="34" t="s">
         <v>87</v>
@@ -11810,7 +11828,7 @@
         <v>318</v>
       </c>
       <c r="L197" s="34" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M197" s="46"/>
       <c r="N197" s="46"/>
@@ -16791,7 +16809,7 @@
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K54 K57 K63:K219</xm:sqref>
+          <xm:sqref>K10:K54 K57 K61:K219</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19038,27 +19056,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19316,32 +19313,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EEA2CD4-B321-4AF0-BAC8-6887893E697D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19358,4 +19351,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
richiesta di accreditamento RSA A1#111#WERFENXX, aggiornamento file report-checklist.xlsx
Buongiorno,

a seguito della comunicazione ricevuta in data 11/07/2025, risottomettiamo la check-list dopo aver rivisto, per i casi di test con ID [52, 53, 55], la compilazione della colonna “R – Invio manuale del documento a FSE a seguito della risoluzione dell’errore”, rendendola coerente con quanto riportato in colonna “S – gestione errore”.

commonName: A1#111#WERFENXX
subject_application_id: parmagts
subject_application_vendor: instrumentation-laboratory-spa
subject_application_version: 12

Attendiamo vostro riscontro.

Grazie.
Cordialmente,

daniele
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#WERFENXX/instrumentation-laboratory-spa/parmagts/12/report-checklist.xlsx
+++ b/GATEWAY/A1#111#WERFENXX/instrumentation-laboratory-spa/parmagts/12/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgrandi\OneDrive - Werfen\Documentos\_IMPIANTI\TORINO\TO4 FSE\FSE Accreditamento LAB\A1#111#WERFENXX\instrumentation-laboratory-spa\parmagts\12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B860C705-C793-49CB-B97E-8658113E1A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0B1581-2E26-4721-8682-AB2F2F01F16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4424,10 +4424,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I58" sqref="I58"/>
+      <selection pane="bottomRight" activeCell="R58" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6534,7 +6534,7 @@
         <v>87</v>
       </c>
       <c r="R55" s="34" t="s">
-        <v>307</v>
+        <v>87</v>
       </c>
       <c r="S55" s="34" t="s">
         <v>503</v>
@@ -6597,7 +6597,7 @@
         <v>87</v>
       </c>
       <c r="R56" s="34" t="s">
-        <v>307</v>
+        <v>87</v>
       </c>
       <c r="S56" s="34" t="s">
         <v>503</v>
@@ -6701,7 +6701,7 @@
         <v>87</v>
       </c>
       <c r="R58" s="34" t="s">
-        <v>307</v>
+        <v>87</v>
       </c>
       <c r="S58" s="34" t="s">
         <v>503</v>
@@ -19306,12 +19306,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19573,21 +19576,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19612,18 +19621,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>